<commit_message>
updated Main sheet, stmt of CFs, DCF using FCF
</commit_message>
<xml_diff>
--- a/TGT.xlsx
+++ b/TGT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\William S\Documents\Models Backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286B25ED-3F50-425A-B75A-443148DE4282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0DDA9F-3BEA-41C6-986D-3FFBD5BEC20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D3FA88B4-C151-4007-87D5-293FBDCB5EFE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D3FA88B4-C151-4007-87D5-293FBDCB5EFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="142">
   <si>
     <t>Company</t>
   </si>
@@ -496,6 +496,12 @@
   </si>
   <si>
     <t>FCF Y/Y</t>
+  </si>
+  <si>
+    <t>Average DCF Price</t>
+  </si>
+  <si>
+    <t>Current Price</t>
   </si>
 </sst>
 </file>
@@ -821,7 +827,37 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="31">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1385,7 +1421,7 @@
     <v>TARGET CORPORATION</v>
     <v>TARGET CORPORATION</v>
     <v>160</v>
-    <v>13.2149</v>
+    <v>13.543200000000001</v>
     <v>159.41999999999999</v>
     <v>163.38</v>
     <v>163.35</v>
@@ -1978,10 +2014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AD8FB6-9B3F-4613-8123-B39F0D5EDE91}">
-  <dimension ref="B3:J11"/>
+  <dimension ref="B3:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1996,10 +2032,13 @@
     <col min="8" max="8" width="9.140625" style="1"/>
     <col min="9" max="9" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
+    <col min="12" max="12" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
@@ -2018,8 +2057,15 @@
         <v>138</v>
       </c>
       <c r="J3" s="45"/>
+      <c r="L3" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="M3" s="10">
+        <f>AVERAGE(G9,J9)</f>
+        <v>275.23201548529039</v>
+      </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4" s="18" t="s">
         <v>2</v>
       </c>
@@ -2043,8 +2089,15 @@
         <f>DCF!AT32</f>
         <v>-0.01</v>
       </c>
+      <c r="L4" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="M4" s="44">
+        <f>C4</f>
+        <v>163.38</v>
+      </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" s="18" t="s">
         <v>3</v>
       </c>
@@ -2069,8 +2122,15 @@
         <f>DCF!AT33</f>
         <v>5.3850700241781214E-2</v>
       </c>
+      <c r="L5" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="M5" s="4">
+        <f>(M3-M4)/M4</f>
+        <v>0.68461265445764719</v>
+      </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" s="18" t="s">
         <v>5</v>
       </c>
@@ -2095,7 +2155,7 @@
         <v>190632.20847372137</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" s="18" t="s">
         <v>6</v>
       </c>
@@ -2121,7 +2181,7 @@
         <v>-13356</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B8" s="18" t="s">
         <v>7</v>
       </c>
@@ -2148,7 +2208,7 @@
         <v>177276.20847372137</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B9" s="22" t="s">
         <v>8</v>
       </c>
@@ -2173,7 +2233,7 @@
         <v>378.95726480060148</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="F10" s="46" t="s">
         <v>62</v>
       </c>
@@ -2189,7 +2249,7 @@
         <v>163.38</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="F11" s="50" t="s">
         <v>63</v>
       </c>
@@ -2207,6 +2267,14 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="M5 J11 G11">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2215,11 +2283,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5CA5FFC-C2FB-4DA3-BA4F-61AACB691A05}">
   <dimension ref="A1:PH100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="ON64" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="AH15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AQ35" sqref="AQ35"/>
+      <selection pane="bottomRight" activeCell="AZ31" sqref="AZ31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -13457,26 +13525,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AQ39">
-    <cfRule type="cellIs" dxfId="27" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32:Z37">
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT39">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>